<commit_message>
Update Cronograma Actividades do Projecto POO2.xlsx
Actualizei o cronograma do projecto de POO2
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
+++ b/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
@@ -39,22 +39,22 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Construir  Interfaces de cadastro e consulta do Animal,Vacina e Cliente</t>
-  </si>
-  <si>
     <t>Construir  Interfaces dos servicos Vacinacao, Exames e Cirurgia</t>
   </si>
   <si>
-    <t>Construir Classe Controller  Animal,Vacina e Cliente</t>
-  </si>
-  <si>
-    <t>Construitr classes DAO e fazer Conexao BD das classes   Animal,Vacina e Cliente</t>
-  </si>
-  <si>
     <t>Construir Classe Controller   Vacinacao, Exames e Cirurgia</t>
   </si>
   <si>
     <t>Construitr classes DAO e fazer Conexao BD das classes  Vacinacao, Exames e Cirurgia</t>
+  </si>
+  <si>
+    <t>Construir Classe Controller  Animal,Vacina , Cliente  e veterinaria</t>
+  </si>
+  <si>
+    <t>Construitr classes DAO e fazer Conexao BD das classes   Animal,Vacina , Cliente e veterinaria</t>
+  </si>
+  <si>
+    <t>Construir  Interfaces de cadastro e consulta do Animal,Vacina , Cliente e veterinaria  (interface update)</t>
   </si>
 </sst>
 </file>
@@ -364,7 +364,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -381,8 +381,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" customWidth="1"/>
+    <col min="2" max="2" width="92.42578125" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -412,7 +412,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -420,7 +420,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -428,7 +428,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -436,7 +436,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -444,7 +444,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,7 +452,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fiz a proposta de desnormalizacao da BD
Proposta de desnormalizacao da BD2
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
+++ b/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Prioridade</t>
   </si>
@@ -30,31 +30,37 @@
     <t>Construir classe Model Simples</t>
   </si>
   <si>
-    <t>Fazer a insercao, actualizacao e eliminacao  de dados</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Construir  Interfaces dos servicos Vacinacao, Exames e Cirurgia</t>
-  </si>
-  <si>
-    <t>Construir Classe Controller   Vacinacao, Exames e Cirurgia</t>
-  </si>
-  <si>
-    <t>Construitr classes DAO e fazer Conexao BD das classes  Vacinacao, Exames e Cirurgia</t>
-  </si>
-  <si>
-    <t>Construir Classe Controller  Animal,Vacina , Cliente  e veterinaria</t>
-  </si>
-  <si>
-    <t>Construitr classes DAO e fazer Conexao BD das classes   Animal,Vacina , Cliente e veterinaria</t>
-  </si>
-  <si>
-    <t>Construir  Interfaces de cadastro e consulta do Animal,Vacina , Cliente e veterinaria  (interface update)</t>
+    <t>Construir  Interfaces de cadastro e consulta Animal (Valter)</t>
+  </si>
+  <si>
+    <t>Construir  Interfaces dos servicos Vacinacao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construir  Interfaces dos servicos Exames </t>
+  </si>
+  <si>
+    <t>Construir  Interfaces dos servicos cirurgia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazer a insercao, actualizacao e eliminacao  de varios dados </t>
+  </si>
+  <si>
+    <t>Fazer relatorios</t>
+  </si>
+  <si>
+    <t>Construir  Interfaces do historico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tela de login (Senha) </t>
+  </si>
+  <si>
+    <t>Construir  Interfaces de cadastro e consulta Cliente  (Jaime) falta Deletar</t>
   </si>
 </sst>
 </file>
@@ -364,7 +370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -372,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +399,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -404,7 +410,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -412,7 +418,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -420,7 +426,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -428,7 +434,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -436,7 +442,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -444,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -452,7 +458,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -460,7 +466,23 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizei a consulta e cadastro do animal
A classe Animal ja registra e consulta os seus dados, so faltar poder ver o resultado dessa consula
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
+++ b/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
@@ -36,18 +36,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Construir  Interfaces de cadastro e consulta Animal (Valter)</t>
-  </si>
-  <si>
-    <t>Construir  Interfaces dos servicos Vacinacao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Construir  Interfaces dos servicos Exames </t>
-  </si>
-  <si>
-    <t>Construir  Interfaces dos servicos cirurgia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fazer a insercao, actualizacao e eliminacao  de varios dados </t>
   </si>
   <si>
@@ -61,6 +49,18 @@
   </si>
   <si>
     <t>Construir  Interfaces de cadastro e consulta Cliente  (Jaime) falta Deletar</t>
+  </si>
+  <si>
+    <t>Construir  Interfaces dos servicos Vacinacao ( Valter)</t>
+  </si>
+  <si>
+    <t>Construir  Interfaces dos servicos cirurgia  ( Valter)</t>
+  </si>
+  <si>
+    <t>Construir  Interfaces dos servicos Exames  (Jaime)</t>
+  </si>
+  <si>
+    <t>Construir  Interfaces de cadastro e consulta Animal (Jaime e valter)</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -418,7 +418,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -426,7 +426,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -434,7 +434,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,7 +442,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,7 +450,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,7 +458,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -466,7 +466,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -474,7 +474,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -482,7 +482,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizei a proposta de particionamentos vertical e horizontal
Actualizei as propostas de particionamento vertical e horizontal
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
+++ b/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Prioridade</t>
   </si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">Tela de login (Senha) </t>
   </si>
   <si>
-    <t>Construir  Interfaces de cadastro e consulta Cliente  (Jaime) falta Deletar</t>
-  </si>
-  <si>
     <t>Construir  Interfaces dos servicos Vacinacao ( Valter)</t>
   </si>
   <si>
@@ -60,7 +57,10 @@
     <t>Construir  Interfaces dos servicos Exames  (Jaime)</t>
   </si>
   <si>
-    <t>Construir  Interfaces de cadastro e consulta Animal (Jaime e valter)</t>
+    <t>Construir  Interfaces de cadastro e consulta Animal (Jaime e valter) falta actualizar dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construir  Interfaces de cadastro e consulta Cliente  (Jaime) </t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +418,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -426,7 +429,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -434,7 +437,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -442,7 +445,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,7 +453,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Conclui a Actualizacao das classe Animal e cliente
As classes animal e cliente ja fazem todo o CRUD
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
+++ b/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Prioridade</t>
   </si>
@@ -36,18 +36,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t xml:space="preserve">Fazer a insercao, actualizacao e eliminacao  de varios dados </t>
-  </si>
-  <si>
-    <t>Fazer relatorios</t>
-  </si>
-  <si>
-    <t>Construir  Interfaces do historico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tela de login (Senha) </t>
-  </si>
-  <si>
     <t>Construir  Interfaces dos servicos Vacinacao ( Valter)</t>
   </si>
   <si>
@@ -57,10 +45,25 @@
     <t>Construir  Interfaces dos servicos Exames  (Jaime)</t>
   </si>
   <si>
-    <t>Construir  Interfaces de cadastro e consulta Animal (Jaime e valter) falta actualizar dados</t>
-  </si>
-  <si>
     <t xml:space="preserve">Construir  Interfaces de cadastro e consulta Cliente  (Jaime) </t>
+  </si>
+  <si>
+    <t>Construir  Interfaces do historico ( Jaime)</t>
+  </si>
+  <si>
+    <t>Fazer relatorios ( Jaime e Valter)</t>
+  </si>
+  <si>
+    <t>Tela de login (Senha)  (Jaime)</t>
+  </si>
+  <si>
+    <t>Tela de Loading (Valter)</t>
+  </si>
+  <si>
+    <t>Fazer a insercao, actualizacao e eliminacao  de varios dados  (Jaime e Valter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Construir  Interfaces de cadastro e consulta Animal (Jaime ) </t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +421,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -429,7 +432,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,7 +443,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -445,7 +451,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -453,7 +459,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -461,7 +467,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -469,7 +475,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -477,7 +483,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -485,7 +491,15 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacao dos documento de BD
Actualizeidos  os documento de BD
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
+++ b/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
@@ -373,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -384,7 +384,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Trabalhei na classe Exame
Criacao da classe Exame
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
+++ b/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
@@ -373,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -384,7 +384,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualizei a localizacao das pastas
Actualizei a localizacao da pastas dos projectos de BD e POO@
</commit_message>
<xml_diff>
--- a/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
+++ b/Documentos Base de dados/Cronograma Actividades do Projecto POO2.xlsx
@@ -45,18 +45,12 @@
     <t xml:space="preserve">Construir  Interfaces de cadastro e consulta Cliente  (Jaime) </t>
   </si>
   <si>
-    <t>Fazer relatorios ( Jaime e Valter)</t>
-  </si>
-  <si>
     <t>Fazer a insercao, actualizacao e eliminacao  de varios dados  (Jaime e Valter)</t>
   </si>
   <si>
     <t xml:space="preserve">Construir  Interfaces de cadastro e consulta Animal (Jaime ) </t>
   </si>
   <si>
-    <t>Construir  Interfaces do historico [ Exame, Vacinacao, Exame ] ( Jaime)</t>
-  </si>
-  <si>
     <t>Construir  Interfaces dos servicos Vacinacao ( Jaime)</t>
   </si>
   <si>
@@ -64,6 +58,12 @@
   </si>
   <si>
     <t>Tela de login (Senha)  (Valter)</t>
+  </si>
+  <si>
+    <t>Construir  Interfaces de relatorios [Cadastro, Servicos e Financeiro] ( Jaime)</t>
+  </si>
+  <si>
+    <t>Gerar relatorios (Jaime)</t>
   </si>
 </sst>
 </file>
@@ -373,7 +373,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -443,7 +443,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -473,7 +473,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -489,7 +489,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -505,7 +505,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>